<commit_message>
feature: update get mysql info
</commit_message>
<xml_diff>
--- a/equipment_sequence/chang_fei/jin_sha_jiang/jin_sha_jiang_manual.xlsx
+++ b/equipment_sequence/chang_fei/jin_sha_jiang/jin_sha_jiang_manual.xlsx
@@ -7785,9 +7785,9 @@
   <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
+      <selection pane="bottomLeft" activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>

</xml_diff>

<commit_message>
feature: update passive-equipment dependency
</commit_message>
<xml_diff>
--- a/equipment_sequence/chang_fei/jin_sha_jiang/jin_sha_jiang_manual.xlsx
+++ b/equipment_sequence/chang_fei/jin_sha_jiang/jin_sha_jiang_manual.xlsx
@@ -92,6 +92,135 @@
         </r>
       </text>
     </comment>
+    <comment ref="B5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>S6F11 W
+  &lt;L [3]
+    &lt;U1 1 &gt;
+    &lt;U2 1003 &gt;
+    &lt;L [1]
+      &lt;L [2]
+        &lt;U4 3 &gt;
+        &lt;L [1]
+          &lt;A "ddddddd"&gt;
+        &gt;
+      &gt;
+    &gt;
+  &gt; .</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>S6F11 W
+  &lt;L [3]
+    &lt;U1 1 &gt;
+    &lt;U2 1004 &gt;
+    &lt;L [1]
+      &lt;L [2]
+        &lt;U4 4 &gt;
+        &lt;L [16]
+          &lt;A&gt;
+          &lt;L [2]
+            &lt;A&gt;
+            &lt;A&gt;
+          &gt;
+          &lt;L [2]
+            &lt;U4 0 &gt;
+            &lt;U4 0 &gt;
+          &gt;
+          &lt;F4 0.0 &gt;
+          &lt;L [4]
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+          &gt;
+          &lt;L [4]
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+          &gt;
+          &lt;L [4]
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+          &gt;
+          &lt;L [4]
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+          &gt;
+          &lt;L [4]
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+          &gt;
+          &lt;L [4]
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+          &gt;
+          &lt;L [4]
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+          &gt;
+          &lt;L [4]
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+          &gt;
+          &lt;L [4]
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+          &gt;
+          &lt;L [4]
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+          &gt;
+          &lt;L [4]
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+          &gt;
+          &lt;L [4]
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+            &lt;F4 0.0 &gt;
+          &gt;
+        &gt;
+      &gt;
+    &gt;
+  &gt; .</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B23" authorId="0">
       <text>
         <r>
@@ -133,6 +262,67 @@
         &lt;U4 2 &gt;
         &lt;L [1]
           &lt;B 0x4&gt;
+        &gt;
+      &gt;
+    &gt;
+  &gt; .</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B25" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">S6F11 W
+  &lt;L [3]
+    &lt;U1 1 &gt;
+    &lt;U2 1003 &gt;
+    &lt;L [1]
+      &lt;L [2]
+        &lt;U4 3 &gt;
+        &lt;L [1]
+          &lt;A "JSJ01-TWELD-T-A-005"&gt;
+        &gt;
+      &gt;
+    &gt;
+  &gt; .
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B26" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>S6F11 W
+  &lt;L [3]
+    &lt;U1 1 &gt;
+    &lt;U2 1004 &gt;
+    &lt;L [1]
+      &lt;L [2]
+        &lt;U4 4 &gt;
+        &lt;L [4]
+          &lt;A&gt;
+          &lt;L [2]
+            &lt;A "product_code_1"&gt;
+            &lt;A "product_code_2"&gt;
+          &gt;
+          &lt;L [2]
+            &lt;A "frame_code_1"&gt;
+            &lt;A "frame_code_2"&gt;
+          &gt;
+          &lt;L [2]
+            &lt;U4 1 &gt;
+            &lt;U4 1 &gt;
+          &gt;
         &gt;
       &gt;
     &gt;
@@ -2629,7 +2819,7 @@
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0_ "/>
   </numFmts>
-  <fonts count="42">
+  <fonts count="41">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2721,13 +2911,6 @@
       <color theme="1"/>
       <name val="黑体"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
@@ -2922,7 +3105,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="49">
+  <fills count="46">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3081,12 +3264,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -3100,18 +3277,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3644,137 +3809,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="25" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="25" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="5" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="5" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="22" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="22" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4022,7 +4187,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4031,154 +4196,142 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="15" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="16" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="16" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="19" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4540,7 +4693,7 @@
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
@@ -4576,13 +4729,13 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="136" t="s">
+      <c r="A2" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="136" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="136" t="s">
+      <c r="B2" s="132" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="132" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="84" t="s">
@@ -4596,13 +4749,13 @@
       </c>
     </row>
     <row r="3" ht="27" spans="1:7">
-      <c r="A3" s="136" t="s">
+      <c r="A3" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="136" t="s">
+      <c r="B3" s="132" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="136" t="s">
+      <c r="C3" s="132" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="84" t="s">
@@ -4611,18 +4764,18 @@
       <c r="F3" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="117" t="s">
+      <c r="G3" s="116" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" ht="40.5" spans="1:7">
-      <c r="A4" s="136" t="s">
+      <c r="A4" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="136" t="s">
+      <c r="B4" s="132" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="136" t="s">
+      <c r="C4" s="132" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="84" t="s">
@@ -4631,18 +4784,18 @@
       <c r="F4" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="117" t="s">
+      <c r="G4" s="116" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" ht="67.5" spans="1:7">
-      <c r="A5" s="136" t="s">
+      <c r="A5" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="136" t="s">
+      <c r="B5" s="132" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="136" t="s">
+      <c r="C5" s="132" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="84" t="s">
@@ -4651,7 +4804,7 @@
       <c r="F5" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="117" t="s">
+      <c r="G5" s="116" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4679,21 +4832,21 @@
       <c r="F7" s="84" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="117" t="s">
+      <c r="G7" s="116" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="84"/>
       <c r="B8" s="84"/>
-      <c r="C8" s="117"/>
+      <c r="C8" s="116"/>
       <c r="E8" s="84" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="84" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="117" t="s">
+      <c r="G8" s="116" t="s">
         <v>26</v>
       </c>
     </row>
@@ -4733,7 +4886,7 @@
       <c r="F10" s="84" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="117" t="s">
+      <c r="G10" s="116" t="s">
         <v>34</v>
       </c>
     </row>
@@ -6089,66 +6242,66 @@
   <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
+      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="6.66666666666667" style="81" customWidth="1"/>
-    <col min="2" max="2" width="25.1083333333333" style="109" customWidth="1"/>
-    <col min="3" max="3" width="21.975" style="109" customWidth="1"/>
+    <col min="2" max="2" width="25.1083333333333" style="108" customWidth="1"/>
+    <col min="3" max="3" width="21.975" style="108" customWidth="1"/>
     <col min="4" max="4" width="10.775" style="81" customWidth="1"/>
     <col min="5" max="5" width="13.1083333333333" style="81" customWidth="1"/>
-    <col min="6" max="6" width="34" style="109" customWidth="1"/>
+    <col min="6" max="6" width="34" style="108" customWidth="1"/>
     <col min="7" max="7" width="16" style="81" customWidth="1"/>
-    <col min="8" max="8" width="39.2333333333333" style="109" customWidth="1"/>
-    <col min="9" max="9" width="28.3583333333333" style="109" customWidth="1"/>
+    <col min="8" max="8" width="39.2333333333333" style="108" customWidth="1"/>
+    <col min="9" max="9" width="28.3583333333333" style="108" customWidth="1"/>
     <col min="10" max="16384" width="9" style="81"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1" spans="1:9">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="120" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="124" t="s">
+      <c r="B1" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="124" t="s">
+      <c r="C1" s="122" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="121" t="s">
+      <c r="D1" s="120" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="121" t="s">
+      <c r="E1" s="120" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="124" t="s">
+      <c r="F1" s="122" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="121" t="s">
+      <c r="G1" s="120" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="124" t="s">
+      <c r="H1" s="122" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="133" t="s">
+      <c r="I1" s="130" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" s="123" customFormat="1" ht="18.75" customHeight="1" spans="1:9">
-      <c r="A2" s="110" t="s">
+    <row r="2" s="107" customFormat="1" ht="18.75" customHeight="1" spans="1:9">
+      <c r="A2" s="109" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="125"/>
-      <c r="C2" s="113"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="134"/>
+      <c r="B2" s="123"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="112"/>
+      <c r="I2" s="131"/>
     </row>
     <row r="3" ht="56.25" spans="1:9">
       <c r="A3" s="105">
@@ -6236,19 +6389,19 @@
       <c r="I5" s="106"/>
     </row>
     <row r="6" ht="18.75" spans="1:9">
-      <c r="A6" s="126">
+      <c r="A6" s="115">
         <v>1004</v>
       </c>
-      <c r="B6" s="127" t="s">
+      <c r="B6" s="124" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="127" t="s">
+      <c r="C6" s="124" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="126">
-        <v>4</v>
-      </c>
-      <c r="E6" s="114">
+      <c r="D6" s="115">
+        <v>4</v>
+      </c>
+      <c r="E6" s="113">
         <v>602</v>
       </c>
       <c r="F6" s="106" t="s">
@@ -6263,30 +6416,30 @@
       <c r="I6" s="106"/>
     </row>
     <row r="7" ht="18.75" spans="1:9">
-      <c r="A7" s="128"/>
-      <c r="B7" s="129"/>
-      <c r="C7" s="129"/>
-      <c r="D7" s="128"/>
-      <c r="E7" s="114">
+      <c r="A7" s="125"/>
+      <c r="B7" s="126"/>
+      <c r="C7" s="126"/>
+      <c r="D7" s="125"/>
+      <c r="E7" s="113">
         <v>607</v>
       </c>
       <c r="F7" s="106" t="s">
         <v>65</v>
       </c>
-      <c r="G7" s="116" t="s">
+      <c r="G7" s="115" t="s">
         <v>66</v>
       </c>
       <c r="H7" s="106" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="117"/>
+      <c r="I7" s="116"/>
     </row>
     <row r="8" ht="37.5" spans="1:9">
-      <c r="A8" s="128"/>
-      <c r="B8" s="129"/>
-      <c r="C8" s="129"/>
-      <c r="D8" s="128"/>
-      <c r="E8" s="114">
+      <c r="A8" s="125"/>
+      <c r="B8" s="126"/>
+      <c r="C8" s="126"/>
+      <c r="D8" s="125"/>
+      <c r="E8" s="113">
         <v>608</v>
       </c>
       <c r="F8" s="106" t="s">
@@ -6298,17 +6451,17 @@
       <c r="H8" s="106" t="s">
         <v>69</v>
       </c>
-      <c r="I8" s="117"/>
+      <c r="I8" s="116"/>
     </row>
     <row r="9" ht="18.75" spans="1:9">
-      <c r="A9" s="128"/>
-      <c r="B9" s="129"/>
-      <c r="C9" s="129"/>
-      <c r="D9" s="128"/>
-      <c r="E9" s="114">
+      <c r="A9" s="125"/>
+      <c r="B9" s="126"/>
+      <c r="C9" s="126"/>
+      <c r="D9" s="125"/>
+      <c r="E9" s="113">
         <v>621</v>
       </c>
-      <c r="F9" s="130" t="s">
+      <c r="F9" s="127" t="s">
         <v>70</v>
       </c>
       <c r="G9" s="105" t="s">
@@ -6317,17 +6470,17 @@
       <c r="H9" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="I9" s="117"/>
+      <c r="I9" s="116"/>
     </row>
     <row r="10" ht="18.75" spans="1:9">
-      <c r="A10" s="128"/>
-      <c r="B10" s="129"/>
-      <c r="C10" s="129"/>
-      <c r="D10" s="128"/>
-      <c r="E10" s="114">
+      <c r="A10" s="125"/>
+      <c r="B10" s="126"/>
+      <c r="C10" s="126"/>
+      <c r="D10" s="125"/>
+      <c r="E10" s="113">
         <v>609</v>
       </c>
-      <c r="F10" s="130" t="s">
+      <c r="F10" s="127" t="s">
         <v>73</v>
       </c>
       <c r="G10" s="105" t="s">
@@ -6336,17 +6489,17 @@
       <c r="H10" s="106" t="s">
         <v>74</v>
       </c>
-      <c r="I10" s="117"/>
+      <c r="I10" s="116"/>
     </row>
     <row r="11" ht="18.75" spans="1:9">
-      <c r="A11" s="128"/>
-      <c r="B11" s="129"/>
-      <c r="C11" s="129"/>
-      <c r="D11" s="128"/>
-      <c r="E11" s="114">
+      <c r="A11" s="125"/>
+      <c r="B11" s="126"/>
+      <c r="C11" s="126"/>
+      <c r="D11" s="125"/>
+      <c r="E11" s="113">
         <v>610</v>
       </c>
-      <c r="F11" s="130" t="s">
+      <c r="F11" s="127" t="s">
         <v>75</v>
       </c>
       <c r="G11" s="105" t="s">
@@ -6355,17 +6508,17 @@
       <c r="H11" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="I11" s="117"/>
+      <c r="I11" s="116"/>
     </row>
     <row r="12" ht="18.75" spans="1:9">
-      <c r="A12" s="128"/>
-      <c r="B12" s="129"/>
-      <c r="C12" s="129"/>
-      <c r="D12" s="128"/>
-      <c r="E12" s="114">
+      <c r="A12" s="125"/>
+      <c r="B12" s="126"/>
+      <c r="C12" s="126"/>
+      <c r="D12" s="125"/>
+      <c r="E12" s="113">
         <v>611</v>
       </c>
-      <c r="F12" s="130" t="s">
+      <c r="F12" s="127" t="s">
         <v>77</v>
       </c>
       <c r="G12" s="105" t="s">
@@ -6374,17 +6527,17 @@
       <c r="H12" s="106" t="s">
         <v>78</v>
       </c>
-      <c r="I12" s="117"/>
+      <c r="I12" s="116"/>
     </row>
     <row r="13" ht="18.75" spans="1:9">
-      <c r="A13" s="128"/>
-      <c r="B13" s="129"/>
-      <c r="C13" s="129"/>
-      <c r="D13" s="128"/>
-      <c r="E13" s="114">
+      <c r="A13" s="125"/>
+      <c r="B13" s="126"/>
+      <c r="C13" s="126"/>
+      <c r="D13" s="125"/>
+      <c r="E13" s="113">
         <v>612</v>
       </c>
-      <c r="F13" s="130" t="s">
+      <c r="F13" s="127" t="s">
         <v>79</v>
       </c>
       <c r="G13" s="105" t="s">
@@ -6393,17 +6546,17 @@
       <c r="H13" s="106" t="s">
         <v>80</v>
       </c>
-      <c r="I13" s="117"/>
+      <c r="I13" s="116"/>
     </row>
     <row r="14" ht="18.75" spans="1:9">
-      <c r="A14" s="128"/>
-      <c r="B14" s="129"/>
-      <c r="C14" s="129"/>
-      <c r="D14" s="128"/>
-      <c r="E14" s="114">
+      <c r="A14" s="125"/>
+      <c r="B14" s="126"/>
+      <c r="C14" s="126"/>
+      <c r="D14" s="125"/>
+      <c r="E14" s="113">
         <v>613</v>
       </c>
-      <c r="F14" s="130" t="s">
+      <c r="F14" s="127" t="s">
         <v>81</v>
       </c>
       <c r="G14" s="105" t="s">
@@ -6412,17 +6565,17 @@
       <c r="H14" s="106" t="s">
         <v>82</v>
       </c>
-      <c r="I14" s="117"/>
+      <c r="I14" s="116"/>
     </row>
     <row r="15" ht="18.75" spans="1:9">
-      <c r="A15" s="128"/>
-      <c r="B15" s="129"/>
-      <c r="C15" s="129"/>
-      <c r="D15" s="128"/>
-      <c r="E15" s="114">
+      <c r="A15" s="125"/>
+      <c r="B15" s="126"/>
+      <c r="C15" s="126"/>
+      <c r="D15" s="125"/>
+      <c r="E15" s="113">
         <v>614</v>
       </c>
-      <c r="F15" s="130" t="s">
+      <c r="F15" s="127" t="s">
         <v>83</v>
       </c>
       <c r="G15" s="105" t="s">
@@ -6431,17 +6584,17 @@
       <c r="H15" s="106" t="s">
         <v>84</v>
       </c>
-      <c r="I15" s="117"/>
+      <c r="I15" s="116"/>
     </row>
     <row r="16" ht="18.75" spans="1:9">
-      <c r="A16" s="128"/>
-      <c r="B16" s="129"/>
-      <c r="C16" s="129"/>
-      <c r="D16" s="128"/>
-      <c r="E16" s="114">
+      <c r="A16" s="125"/>
+      <c r="B16" s="126"/>
+      <c r="C16" s="126"/>
+      <c r="D16" s="125"/>
+      <c r="E16" s="113">
         <v>615</v>
       </c>
-      <c r="F16" s="130" t="s">
+      <c r="F16" s="127" t="s">
         <v>85</v>
       </c>
       <c r="G16" s="105" t="s">
@@ -6450,17 +6603,17 @@
       <c r="H16" s="106" t="s">
         <v>86</v>
       </c>
-      <c r="I16" s="117"/>
+      <c r="I16" s="116"/>
     </row>
     <row r="17" ht="18.75" spans="1:9">
-      <c r="A17" s="128"/>
-      <c r="B17" s="129"/>
-      <c r="C17" s="129"/>
-      <c r="D17" s="128"/>
-      <c r="E17" s="114">
+      <c r="A17" s="125"/>
+      <c r="B17" s="126"/>
+      <c r="C17" s="126"/>
+      <c r="D17" s="125"/>
+      <c r="E17" s="113">
         <v>616</v>
       </c>
-      <c r="F17" s="130" t="s">
+      <c r="F17" s="127" t="s">
         <v>87</v>
       </c>
       <c r="G17" s="105" t="s">
@@ -6469,17 +6622,17 @@
       <c r="H17" s="106" t="s">
         <v>88</v>
       </c>
-      <c r="I17" s="117"/>
+      <c r="I17" s="116"/>
     </row>
     <row r="18" ht="18.75" spans="1:9">
-      <c r="A18" s="128"/>
-      <c r="B18" s="129"/>
-      <c r="C18" s="129"/>
-      <c r="D18" s="128"/>
-      <c r="E18" s="114">
+      <c r="A18" s="125"/>
+      <c r="B18" s="126"/>
+      <c r="C18" s="126"/>
+      <c r="D18" s="125"/>
+      <c r="E18" s="113">
         <v>617</v>
       </c>
-      <c r="F18" s="130" t="s">
+      <c r="F18" s="127" t="s">
         <v>89</v>
       </c>
       <c r="G18" s="105" t="s">
@@ -6488,17 +6641,17 @@
       <c r="H18" s="106" t="s">
         <v>90</v>
       </c>
-      <c r="I18" s="117"/>
+      <c r="I18" s="116"/>
     </row>
     <row r="19" ht="18.75" spans="1:9">
-      <c r="A19" s="128"/>
-      <c r="B19" s="129"/>
-      <c r="C19" s="129"/>
-      <c r="D19" s="128"/>
-      <c r="E19" s="114">
+      <c r="A19" s="125"/>
+      <c r="B19" s="126"/>
+      <c r="C19" s="126"/>
+      <c r="D19" s="125"/>
+      <c r="E19" s="113">
         <v>618</v>
       </c>
-      <c r="F19" s="130" t="s">
+      <c r="F19" s="127" t="s">
         <v>91</v>
       </c>
       <c r="G19" s="105" t="s">
@@ -6507,17 +6660,17 @@
       <c r="H19" s="106" t="s">
         <v>92</v>
       </c>
-      <c r="I19" s="117"/>
+      <c r="I19" s="116"/>
     </row>
     <row r="20" ht="18.75" spans="1:9">
-      <c r="A20" s="128"/>
-      <c r="B20" s="129"/>
-      <c r="C20" s="129"/>
-      <c r="D20" s="128"/>
-      <c r="E20" s="114">
+      <c r="A20" s="125"/>
+      <c r="B20" s="126"/>
+      <c r="C20" s="126"/>
+      <c r="D20" s="125"/>
+      <c r="E20" s="113">
         <v>619</v>
       </c>
-      <c r="F20" s="130" t="s">
+      <c r="F20" s="127" t="s">
         <v>93</v>
       </c>
       <c r="G20" s="105" t="s">
@@ -6526,17 +6679,17 @@
       <c r="H20" s="106" t="s">
         <v>94</v>
       </c>
-      <c r="I20" s="117"/>
+      <c r="I20" s="116"/>
     </row>
     <row r="21" ht="18.75" spans="1:9">
-      <c r="A21" s="128"/>
-      <c r="B21" s="129"/>
-      <c r="C21" s="129"/>
-      <c r="D21" s="128"/>
-      <c r="E21" s="114">
+      <c r="A21" s="125"/>
+      <c r="B21" s="126"/>
+      <c r="C21" s="126"/>
+      <c r="D21" s="125"/>
+      <c r="E21" s="113">
         <v>620</v>
       </c>
-      <c r="F21" s="130" t="s">
+      <c r="F21" s="127" t="s">
         <v>95</v>
       </c>
       <c r="G21" s="105" t="s">
@@ -6545,13 +6698,13 @@
       <c r="H21" s="106" t="s">
         <v>96</v>
       </c>
-      <c r="I21" s="117"/>
+      <c r="I21" s="116"/>
     </row>
     <row r="22" ht="18.75" spans="1:9">
-      <c r="A22" s="110" t="s">
+      <c r="A22" s="109" t="s">
         <v>97</v>
       </c>
-      <c r="B22" s="125"/>
+      <c r="B22" s="123"/>
       <c r="C22" s="106"/>
       <c r="D22" s="105"/>
       <c r="E22" s="105"/>
@@ -6646,19 +6799,19 @@
       <c r="I25" s="106"/>
     </row>
     <row r="26" ht="18.75" spans="1:9">
-      <c r="A26" s="126">
+      <c r="A26" s="115">
         <v>1004</v>
       </c>
-      <c r="B26" s="127" t="s">
+      <c r="B26" s="124" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="127" t="s">
+      <c r="C26" s="124" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="126">
-        <v>4</v>
-      </c>
-      <c r="E26" s="114">
+      <c r="D26" s="115">
+        <v>4</v>
+      </c>
+      <c r="E26" s="113">
         <v>602</v>
       </c>
       <c r="F26" s="106" t="s">
@@ -6673,33 +6826,33 @@
       <c r="I26" s="106"/>
     </row>
     <row r="27" ht="18.75" spans="1:9">
-      <c r="A27" s="128"/>
-      <c r="B27" s="129"/>
-      <c r="C27" s="129"/>
-      <c r="D27" s="128"/>
-      <c r="E27" s="114">
+      <c r="A27" s="125"/>
+      <c r="B27" s="126"/>
+      <c r="C27" s="126"/>
+      <c r="D27" s="125"/>
+      <c r="E27" s="113">
         <v>607</v>
       </c>
       <c r="F27" s="106" t="s">
         <v>65</v>
       </c>
-      <c r="G27" s="116" t="s">
+      <c r="G27" s="115" t="s">
         <v>66</v>
       </c>
       <c r="H27" s="106" t="s">
         <v>67</v>
       </c>
-      <c r="I27" s="117"/>
+      <c r="I27" s="116"/>
     </row>
     <row r="28" ht="18.75" spans="1:9">
-      <c r="A28" s="128"/>
-      <c r="B28" s="129"/>
-      <c r="C28" s="129"/>
-      <c r="D28" s="128"/>
-      <c r="E28" s="114">
+      <c r="A28" s="125"/>
+      <c r="B28" s="126"/>
+      <c r="C28" s="126"/>
+      <c r="D28" s="125"/>
+      <c r="E28" s="113">
         <v>608</v>
       </c>
-      <c r="F28" s="130" t="s">
+      <c r="F28" s="127" t="s">
         <v>98</v>
       </c>
       <c r="G28" s="105" t="s">
@@ -6708,14 +6861,14 @@
       <c r="H28" s="106" t="s">
         <v>99</v>
       </c>
-      <c r="I28" s="117"/>
+      <c r="I28" s="116"/>
     </row>
     <row r="29" ht="37.5" spans="1:9">
-      <c r="A29" s="131"/>
-      <c r="B29" s="132"/>
-      <c r="C29" s="132"/>
-      <c r="D29" s="131"/>
-      <c r="E29" s="114">
+      <c r="A29" s="128"/>
+      <c r="B29" s="129"/>
+      <c r="C29" s="129"/>
+      <c r="D29" s="128"/>
+      <c r="E29" s="113">
         <v>609</v>
       </c>
       <c r="F29" s="106" t="s">
@@ -6730,10 +6883,10 @@
       <c r="I29" s="106"/>
     </row>
     <row r="30" ht="18.75" spans="1:9">
-      <c r="A30" s="110" t="s">
+      <c r="A30" s="109" t="s">
         <v>100</v>
       </c>
-      <c r="B30" s="125"/>
+      <c r="B30" s="123"/>
       <c r="C30" s="106"/>
       <c r="D30" s="105"/>
       <c r="E30" s="105"/>
@@ -6813,7 +6966,7 @@
       <c r="D33" s="105">
         <v>3</v>
       </c>
-      <c r="E33" s="114">
+      <c r="E33" s="113">
         <v>601</v>
       </c>
       <c r="F33" s="106" t="s">
@@ -6828,19 +6981,19 @@
       <c r="I33" s="106"/>
     </row>
     <row r="34" ht="18.75" spans="1:9">
-      <c r="A34" s="126">
+      <c r="A34" s="115">
         <v>1004</v>
       </c>
-      <c r="B34" s="127" t="s">
+      <c r="B34" s="124" t="s">
         <v>105</v>
       </c>
-      <c r="C34" s="127" t="s">
+      <c r="C34" s="124" t="s">
         <v>106</v>
       </c>
-      <c r="D34" s="126">
-        <v>4</v>
-      </c>
-      <c r="E34" s="114">
+      <c r="D34" s="115">
+        <v>4</v>
+      </c>
+      <c r="E34" s="113">
         <v>603</v>
       </c>
       <c r="F34" s="106" t="s">
@@ -6855,17 +7008,17 @@
       <c r="I34" s="106"/>
     </row>
     <row r="35" ht="18.75" spans="1:9">
-      <c r="A35" s="128"/>
-      <c r="B35" s="129"/>
-      <c r="C35" s="129"/>
-      <c r="D35" s="128"/>
-      <c r="E35" s="114">
+      <c r="A35" s="125"/>
+      <c r="B35" s="126"/>
+      <c r="C35" s="126"/>
+      <c r="D35" s="125"/>
+      <c r="E35" s="113">
         <v>619</v>
       </c>
       <c r="F35" s="106" t="s">
         <v>109</v>
       </c>
-      <c r="G35" s="116" t="s">
+      <c r="G35" s="115" t="s">
         <v>66</v>
       </c>
       <c r="H35" s="106" t="s">
@@ -6874,17 +7027,17 @@
       <c r="I35" s="106"/>
     </row>
     <row r="36" ht="18.75" spans="1:9">
-      <c r="A36" s="128"/>
-      <c r="B36" s="129"/>
-      <c r="C36" s="129"/>
-      <c r="D36" s="128"/>
-      <c r="E36" s="114">
+      <c r="A36" s="125"/>
+      <c r="B36" s="126"/>
+      <c r="C36" s="126"/>
+      <c r="D36" s="125"/>
+      <c r="E36" s="113">
         <v>621</v>
       </c>
       <c r="F36" s="106" t="s">
         <v>111</v>
       </c>
-      <c r="G36" s="116" t="s">
+      <c r="G36" s="115" t="s">
         <v>66</v>
       </c>
       <c r="H36" s="106" t="s">
@@ -6893,99 +7046,99 @@
       <c r="I36" s="106"/>
     </row>
     <row r="37" ht="37.5" spans="1:9">
-      <c r="A37" s="128"/>
-      <c r="B37" s="129"/>
-      <c r="C37" s="129"/>
-      <c r="D37" s="128"/>
-      <c r="E37" s="114">
+      <c r="A37" s="125"/>
+      <c r="B37" s="126"/>
+      <c r="C37" s="126"/>
+      <c r="D37" s="125"/>
+      <c r="E37" s="113">
         <v>623</v>
       </c>
       <c r="F37" s="106" t="s">
         <v>113</v>
       </c>
-      <c r="G37" s="116" t="s">
+      <c r="G37" s="115" t="s">
         <v>66</v>
       </c>
       <c r="H37" s="106" t="s">
         <v>114</v>
       </c>
-      <c r="I37" s="135"/>
+      <c r="I37" s="116"/>
     </row>
     <row r="38" ht="18.75" spans="1:9">
-      <c r="A38" s="128"/>
-      <c r="B38" s="129"/>
-      <c r="C38" s="129"/>
-      <c r="D38" s="128"/>
-      <c r="E38" s="114">
+      <c r="A38" s="125"/>
+      <c r="B38" s="126"/>
+      <c r="C38" s="126"/>
+      <c r="D38" s="125"/>
+      <c r="E38" s="113">
         <v>625</v>
       </c>
       <c r="F38" s="106" t="s">
         <v>115</v>
       </c>
-      <c r="G38" s="116" t="s">
+      <c r="G38" s="115" t="s">
         <v>66</v>
       </c>
       <c r="H38" s="106" t="s">
         <v>116</v>
       </c>
-      <c r="I38" s="135"/>
+      <c r="I38" s="116"/>
     </row>
     <row r="39" ht="18.75" spans="1:9">
-      <c r="A39" s="128"/>
-      <c r="B39" s="129"/>
-      <c r="C39" s="129"/>
-      <c r="D39" s="128"/>
-      <c r="E39" s="114">
+      <c r="A39" s="125"/>
+      <c r="B39" s="126"/>
+      <c r="C39" s="126"/>
+      <c r="D39" s="125"/>
+      <c r="E39" s="113">
         <v>627</v>
       </c>
       <c r="F39" s="106" t="s">
         <v>117</v>
       </c>
-      <c r="G39" s="116" t="s">
+      <c r="G39" s="115" t="s">
         <v>66</v>
       </c>
       <c r="H39" s="106" t="s">
         <v>118</v>
       </c>
-      <c r="I39" s="135"/>
+      <c r="I39" s="116"/>
     </row>
     <row r="40" ht="18.75" spans="1:9">
-      <c r="A40" s="128"/>
-      <c r="B40" s="129"/>
-      <c r="C40" s="129"/>
-      <c r="D40" s="128"/>
-      <c r="E40" s="114">
+      <c r="A40" s="125"/>
+      <c r="B40" s="126"/>
+      <c r="C40" s="126"/>
+      <c r="D40" s="125"/>
+      <c r="E40" s="113">
         <v>629</v>
       </c>
       <c r="F40" s="106" t="s">
         <v>119</v>
       </c>
-      <c r="G40" s="116" t="s">
+      <c r="G40" s="115" t="s">
         <v>66</v>
       </c>
       <c r="H40" s="106" t="s">
         <v>120</v>
       </c>
-      <c r="I40" s="135"/>
+      <c r="I40" s="116"/>
     </row>
     <row r="41" ht="18.75" spans="1:9">
-      <c r="A41" s="131"/>
-      <c r="B41" s="132"/>
-      <c r="C41" s="132"/>
-      <c r="D41" s="131"/>
-      <c r="E41" s="114">
+      <c r="A41" s="128"/>
+      <c r="B41" s="129"/>
+      <c r="C41" s="129"/>
+      <c r="D41" s="128"/>
+      <c r="E41" s="113">
         <v>631</v>
       </c>
       <c r="F41" s="106" t="s">
         <v>121</v>
       </c>
-      <c r="G41" s="116" t="s">
+      <c r="G41" s="115" t="s">
         <v>66</v>
       </c>
       <c r="H41" s="106" t="s">
         <v>122</v>
       </c>
-      <c r="I41" s="135"/>
+      <c r="I41" s="116"/>
     </row>
     <row r="42" ht="37.5" spans="1:9">
       <c r="A42" s="105">
@@ -7000,7 +7153,7 @@
       <c r="D42" s="105">
         <v>5</v>
       </c>
-      <c r="E42" s="114">
+      <c r="E42" s="113">
         <v>602</v>
       </c>
       <c r="F42" s="106" t="s">
@@ -7015,19 +7168,19 @@
       <c r="I42" s="106"/>
     </row>
     <row r="43" ht="18.75" spans="1:9">
-      <c r="A43" s="126">
+      <c r="A43" s="115">
         <v>1006</v>
       </c>
-      <c r="B43" s="127" t="s">
+      <c r="B43" s="124" t="s">
         <v>127</v>
       </c>
-      <c r="C43" s="127" t="s">
+      <c r="C43" s="124" t="s">
         <v>128</v>
       </c>
-      <c r="D43" s="126">
+      <c r="D43" s="115">
         <v>6</v>
       </c>
-      <c r="E43" s="114">
+      <c r="E43" s="113">
         <v>604</v>
       </c>
       <c r="F43" s="106" t="s">
@@ -7042,17 +7195,17 @@
       <c r="I43" s="106"/>
     </row>
     <row r="44" ht="18.75" spans="1:9">
-      <c r="A44" s="128"/>
-      <c r="B44" s="129"/>
-      <c r="C44" s="129"/>
-      <c r="D44" s="128"/>
-      <c r="E44" s="114">
+      <c r="A44" s="125"/>
+      <c r="B44" s="126"/>
+      <c r="C44" s="126"/>
+      <c r="D44" s="125"/>
+      <c r="E44" s="113">
         <v>620</v>
       </c>
       <c r="F44" s="106" t="s">
         <v>131</v>
       </c>
-      <c r="G44" s="116" t="s">
+      <c r="G44" s="115" t="s">
         <v>66</v>
       </c>
       <c r="H44" s="106" t="s">
@@ -7061,17 +7214,17 @@
       <c r="I44" s="106"/>
     </row>
     <row r="45" ht="18.75" spans="1:9">
-      <c r="A45" s="128"/>
-      <c r="B45" s="129"/>
-      <c r="C45" s="129"/>
-      <c r="D45" s="128"/>
-      <c r="E45" s="114">
+      <c r="A45" s="125"/>
+      <c r="B45" s="126"/>
+      <c r="C45" s="126"/>
+      <c r="D45" s="125"/>
+      <c r="E45" s="113">
         <v>622</v>
       </c>
       <c r="F45" s="106" t="s">
         <v>133</v>
       </c>
-      <c r="G45" s="116" t="s">
+      <c r="G45" s="115" t="s">
         <v>66</v>
       </c>
       <c r="H45" s="106" t="s">
@@ -7080,125 +7233,125 @@
       <c r="I45" s="106"/>
     </row>
     <row r="46" ht="37.5" spans="1:9">
-      <c r="A46" s="128"/>
-      <c r="B46" s="129"/>
-      <c r="C46" s="129"/>
-      <c r="D46" s="128"/>
-      <c r="E46" s="114">
+      <c r="A46" s="125"/>
+      <c r="B46" s="126"/>
+      <c r="C46" s="126"/>
+      <c r="D46" s="125"/>
+      <c r="E46" s="113">
         <v>624</v>
       </c>
       <c r="F46" s="106" t="s">
         <v>135</v>
       </c>
-      <c r="G46" s="116" t="s">
+      <c r="G46" s="115" t="s">
         <v>66</v>
       </c>
       <c r="H46" s="106" t="s">
         <v>136</v>
       </c>
-      <c r="I46" s="135"/>
+      <c r="I46" s="116"/>
     </row>
     <row r="47" ht="18.75" spans="1:9">
-      <c r="A47" s="128"/>
-      <c r="B47" s="129"/>
-      <c r="C47" s="129"/>
-      <c r="D47" s="128"/>
-      <c r="E47" s="114">
+      <c r="A47" s="125"/>
+      <c r="B47" s="126"/>
+      <c r="C47" s="126"/>
+      <c r="D47" s="125"/>
+      <c r="E47" s="113">
         <v>626</v>
       </c>
       <c r="F47" s="106" t="s">
         <v>137</v>
       </c>
-      <c r="G47" s="116" t="s">
+      <c r="G47" s="115" t="s">
         <v>66</v>
       </c>
       <c r="H47" s="106" t="s">
         <v>138</v>
       </c>
-      <c r="I47" s="135"/>
+      <c r="I47" s="116"/>
     </row>
     <row r="48" ht="18.75" spans="1:9">
-      <c r="A48" s="128"/>
-      <c r="B48" s="129"/>
-      <c r="C48" s="129"/>
-      <c r="D48" s="128"/>
-      <c r="E48" s="114">
+      <c r="A48" s="125"/>
+      <c r="B48" s="126"/>
+      <c r="C48" s="126"/>
+      <c r="D48" s="125"/>
+      <c r="E48" s="113">
         <v>628</v>
       </c>
       <c r="F48" s="106" t="s">
         <v>139</v>
       </c>
-      <c r="G48" s="116" t="s">
+      <c r="G48" s="115" t="s">
         <v>66</v>
       </c>
       <c r="H48" s="106" t="s">
         <v>140</v>
       </c>
-      <c r="I48" s="135"/>
+      <c r="I48" s="116"/>
     </row>
     <row r="49" ht="18.75" spans="1:9">
-      <c r="A49" s="128"/>
-      <c r="B49" s="129"/>
-      <c r="C49" s="129"/>
-      <c r="D49" s="128"/>
-      <c r="E49" s="114">
+      <c r="A49" s="125"/>
+      <c r="B49" s="126"/>
+      <c r="C49" s="126"/>
+      <c r="D49" s="125"/>
+      <c r="E49" s="113">
         <v>630</v>
       </c>
       <c r="F49" s="106" t="s">
         <v>141</v>
       </c>
-      <c r="G49" s="116" t="s">
+      <c r="G49" s="115" t="s">
         <v>66</v>
       </c>
       <c r="H49" s="106" t="s">
         <v>142</v>
       </c>
-      <c r="I49" s="135"/>
+      <c r="I49" s="116"/>
     </row>
     <row r="50" ht="18.75" spans="1:9">
-      <c r="A50" s="128"/>
-      <c r="B50" s="129"/>
-      <c r="C50" s="129"/>
-      <c r="D50" s="128"/>
-      <c r="E50" s="114">
+      <c r="A50" s="125"/>
+      <c r="B50" s="126"/>
+      <c r="C50" s="126"/>
+      <c r="D50" s="125"/>
+      <c r="E50" s="113">
         <v>632</v>
       </c>
       <c r="F50" s="106" t="s">
         <v>143</v>
       </c>
-      <c r="G50" s="116" t="s">
+      <c r="G50" s="115" t="s">
         <v>66</v>
       </c>
       <c r="H50" s="106" t="s">
         <v>144</v>
       </c>
-      <c r="I50" s="135"/>
+      <c r="I50" s="116"/>
     </row>
     <row r="51" ht="18.75" spans="1:9">
-      <c r="A51" s="128"/>
-      <c r="B51" s="129"/>
-      <c r="C51" s="129"/>
-      <c r="D51" s="128"/>
-      <c r="E51" s="114">
+      <c r="A51" s="125"/>
+      <c r="B51" s="126"/>
+      <c r="C51" s="126"/>
+      <c r="D51" s="125"/>
+      <c r="E51" s="113">
         <v>633</v>
       </c>
       <c r="F51" s="106" t="s">
         <v>145</v>
       </c>
-      <c r="G51" s="116" t="s">
+      <c r="G51" s="115" t="s">
         <v>66</v>
       </c>
       <c r="H51" s="106" t="s">
         <v>146</v>
       </c>
-      <c r="I51" s="135"/>
+      <c r="I51" s="116"/>
     </row>
     <row r="52" ht="18.75" spans="1:9">
-      <c r="A52" s="128"/>
-      <c r="B52" s="129"/>
-      <c r="C52" s="129"/>
-      <c r="D52" s="128"/>
-      <c r="E52" s="114">
+      <c r="A52" s="125"/>
+      <c r="B52" s="126"/>
+      <c r="C52" s="126"/>
+      <c r="D52" s="125"/>
+      <c r="E52" s="113">
         <v>634</v>
       </c>
       <c r="F52" s="106" t="s">
@@ -7210,14 +7363,14 @@
       <c r="H52" s="106" t="s">
         <v>148</v>
       </c>
-      <c r="I52" s="135"/>
+      <c r="I52" s="116"/>
     </row>
     <row r="53" ht="18.75" spans="1:9">
-      <c r="A53" s="131"/>
-      <c r="B53" s="132"/>
-      <c r="C53" s="132"/>
-      <c r="D53" s="131"/>
-      <c r="E53" s="114">
+      <c r="A53" s="128"/>
+      <c r="B53" s="129"/>
+      <c r="C53" s="129"/>
+      <c r="D53" s="128"/>
+      <c r="E53" s="113">
         <v>635</v>
       </c>
       <c r="F53" s="106" t="s">
@@ -7229,7 +7382,7 @@
       <c r="H53" s="106" t="s">
         <v>150</v>
       </c>
-      <c r="I53" s="135"/>
+      <c r="I53" s="116"/>
     </row>
   </sheetData>
   <mergeCells count="19">
@@ -7273,29 +7426,29 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="6.66666666666667" style="120" customWidth="1"/>
-    <col min="2" max="2" width="29.8833333333333" style="120" customWidth="1"/>
-    <col min="3" max="3" width="16" style="120" customWidth="1"/>
-    <col min="4" max="4" width="48.25" style="120" customWidth="1"/>
-    <col min="5" max="5" width="40.775" style="120" customWidth="1"/>
-    <col min="6" max="6" width="22.4416666666667" style="120" customWidth="1"/>
-    <col min="7" max="16384" width="9" style="120"/>
+    <col min="1" max="1" width="6.66666666666667" style="119" customWidth="1"/>
+    <col min="2" max="2" width="29.8833333333333" style="119" customWidth="1"/>
+    <col min="3" max="3" width="16" style="119" customWidth="1"/>
+    <col min="4" max="4" width="48.25" style="119" customWidth="1"/>
+    <col min="5" max="5" width="40.775" style="119" customWidth="1"/>
+    <col min="6" max="6" width="22.4416666666667" style="119" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="119"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="121" t="s">
+      <c r="A1" s="120" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="121" t="s">
+      <c r="B1" s="120" t="s">
         <v>152</v>
       </c>
-      <c r="C1" s="121" t="s">
+      <c r="C1" s="120" t="s">
         <v>153</v>
       </c>
-      <c r="D1" s="121" t="s">
+      <c r="D1" s="120" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="121" t="s">
+      <c r="E1" s="120" t="s">
         <v>154</v>
       </c>
     </row>
@@ -7329,7 +7482,7 @@
       <c r="D3" s="105" t="s">
         <v>54</v>
       </c>
-      <c r="E3" s="122" t="s">
+      <c r="E3" s="121" t="s">
         <v>55</v>
       </c>
     </row>
@@ -7346,7 +7499,7 @@
       <c r="D4" s="105" t="s">
         <v>156</v>
       </c>
-      <c r="E4" s="122"/>
+      <c r="E4" s="121"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="105">
@@ -7361,7 +7514,7 @@
       <c r="D5" s="105" t="s">
         <v>159</v>
       </c>
-      <c r="E5" s="122"/>
+      <c r="E5" s="121"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="105">
@@ -7376,7 +7529,7 @@
       <c r="D6" s="105" t="s">
         <v>161</v>
       </c>
-      <c r="E6" s="122"/>
+      <c r="E6" s="121"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="105">
@@ -7391,7 +7544,7 @@
       <c r="D7" s="106" t="s">
         <v>163</v>
       </c>
-      <c r="E7" s="122"/>
+      <c r="E7" s="121"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="105">
@@ -7406,7 +7559,7 @@
       <c r="D8" s="105" t="s">
         <v>165</v>
       </c>
-      <c r="E8" s="122"/>
+      <c r="E8" s="121"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="105">
@@ -7421,7 +7574,7 @@
       <c r="D9" s="105" t="s">
         <v>167</v>
       </c>
-      <c r="E9" s="122"/>
+      <c r="E9" s="121"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="105">
@@ -7436,7 +7589,7 @@
       <c r="D10" s="105" t="s">
         <v>169</v>
       </c>
-      <c r="E10" s="122"/>
+      <c r="E10" s="121"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="105">
@@ -7451,7 +7604,7 @@
       <c r="D11" s="105" t="s">
         <v>171</v>
       </c>
-      <c r="E11" s="122"/>
+      <c r="E11" s="121"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7473,12 +7626,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="11.3333333333333" style="108" customWidth="1"/>
-    <col min="2" max="2" width="41.625" style="108" customWidth="1"/>
-    <col min="3" max="3" width="13.75" style="108" customWidth="1"/>
-    <col min="4" max="4" width="61.5" style="108" customWidth="1"/>
-    <col min="5" max="5" width="45.3333333333333" style="109" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="108"/>
+    <col min="1" max="1" width="11.3333333333333" style="81" customWidth="1"/>
+    <col min="2" max="2" width="41.625" style="81" customWidth="1"/>
+    <col min="3" max="3" width="13.75" style="81" customWidth="1"/>
+    <col min="4" max="4" width="61.5" style="81" customWidth="1"/>
+    <col min="5" max="5" width="45.3333333333333" style="108" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="81"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" spans="1:5">
@@ -7499,16 +7652,16 @@
       </c>
     </row>
     <row r="2" s="107" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A2" s="110" t="s">
+      <c r="A2" s="109" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="111"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="113"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="112"/>
     </row>
     <row r="3" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A3" s="114">
+      <c r="A3" s="113">
         <v>601</v>
       </c>
       <c r="B3" s="105" t="s">
@@ -7517,13 +7670,13 @@
       <c r="C3" s="105" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="115" t="s">
+      <c r="D3" s="114" t="s">
         <v>175</v>
       </c>
       <c r="E3" s="106"/>
     </row>
     <row r="4" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A4" s="114">
+      <c r="A4" s="113">
         <v>602</v>
       </c>
       <c r="B4" s="105" t="s">
@@ -7538,7 +7691,7 @@
       <c r="E4" s="106"/>
     </row>
     <row r="5" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A5" s="114">
+      <c r="A5" s="113">
         <v>603</v>
       </c>
       <c r="B5" s="105" t="s">
@@ -7553,7 +7706,7 @@
       <c r="E5" s="106"/>
     </row>
     <row r="6" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A6" s="114">
+      <c r="A6" s="113">
         <v>604</v>
       </c>
       <c r="B6" s="105" t="s">
@@ -7568,13 +7721,13 @@
       <c r="E6" s="106"/>
     </row>
     <row r="7" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A7" s="114">
+      <c r="A7" s="113">
         <v>605</v>
       </c>
       <c r="B7" s="105" t="s">
         <v>180</v>
       </c>
-      <c r="C7" s="116" t="s">
+      <c r="C7" s="115" t="s">
         <v>181</v>
       </c>
       <c r="D7" s="105" t="s">
@@ -7583,13 +7736,13 @@
       <c r="E7" s="106"/>
     </row>
     <row r="8" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A8" s="114">
+      <c r="A8" s="113">
         <v>606</v>
       </c>
       <c r="B8" s="105" t="s">
         <v>183</v>
       </c>
-      <c r="C8" s="116" t="s">
+      <c r="C8" s="115" t="s">
         <v>181</v>
       </c>
       <c r="D8" s="105" t="s">
@@ -7598,22 +7751,22 @@
       <c r="E8" s="106"/>
     </row>
     <row r="9" ht="18.75" spans="1:5">
-      <c r="A9" s="114">
+      <c r="A9" s="113">
         <v>607</v>
       </c>
       <c r="B9" s="105" t="s">
         <v>65</v>
       </c>
-      <c r="C9" s="116" t="s">
+      <c r="C9" s="115" t="s">
         <v>66</v>
       </c>
       <c r="D9" s="105" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="117"/>
+      <c r="E9" s="116"/>
     </row>
     <row r="10" ht="18.75" spans="1:5">
-      <c r="A10" s="114">
+      <c r="A10" s="113">
         <v>608</v>
       </c>
       <c r="B10" s="105" t="s">
@@ -7625,13 +7778,13 @@
       <c r="D10" s="105" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="117"/>
+      <c r="E10" s="116"/>
     </row>
     <row r="11" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A11" s="114">
+      <c r="A11" s="113">
         <v>609</v>
       </c>
-      <c r="B11" s="118" t="s">
+      <c r="B11" s="117" t="s">
         <v>73</v>
       </c>
       <c r="C11" s="105" t="s">
@@ -7640,13 +7793,13 @@
       <c r="D11" s="105" t="s">
         <v>74</v>
       </c>
-      <c r="E11" s="117"/>
+      <c r="E11" s="116"/>
     </row>
     <row r="12" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A12" s="114">
+      <c r="A12" s="113">
         <v>610</v>
       </c>
-      <c r="B12" s="118" t="s">
+      <c r="B12" s="117" t="s">
         <v>75</v>
       </c>
       <c r="C12" s="105" t="s">
@@ -7655,13 +7808,13 @@
       <c r="D12" s="105" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="117"/>
+      <c r="E12" s="116"/>
     </row>
     <row r="13" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A13" s="114">
+      <c r="A13" s="113">
         <v>611</v>
       </c>
-      <c r="B13" s="118" t="s">
+      <c r="B13" s="117" t="s">
         <v>77</v>
       </c>
       <c r="C13" s="105" t="s">
@@ -7670,13 +7823,13 @@
       <c r="D13" s="105" t="s">
         <v>78</v>
       </c>
-      <c r="E13" s="117"/>
+      <c r="E13" s="116"/>
     </row>
     <row r="14" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A14" s="114">
+      <c r="A14" s="113">
         <v>612</v>
       </c>
-      <c r="B14" s="118" t="s">
+      <c r="B14" s="117" t="s">
         <v>79</v>
       </c>
       <c r="C14" s="105" t="s">
@@ -7685,13 +7838,13 @@
       <c r="D14" s="105" t="s">
         <v>80</v>
       </c>
-      <c r="E14" s="117"/>
+      <c r="E14" s="116"/>
     </row>
     <row r="15" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A15" s="114">
+      <c r="A15" s="113">
         <v>613</v>
       </c>
-      <c r="B15" s="118" t="s">
+      <c r="B15" s="117" t="s">
         <v>81</v>
       </c>
       <c r="C15" s="105" t="s">
@@ -7700,13 +7853,13 @@
       <c r="D15" s="105" t="s">
         <v>82</v>
       </c>
-      <c r="E15" s="117"/>
+      <c r="E15" s="116"/>
     </row>
     <row r="16" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A16" s="114">
+      <c r="A16" s="113">
         <v>614</v>
       </c>
-      <c r="B16" s="118" t="s">
+      <c r="B16" s="117" t="s">
         <v>83</v>
       </c>
       <c r="C16" s="105" t="s">
@@ -7715,13 +7868,13 @@
       <c r="D16" s="105" t="s">
         <v>84</v>
       </c>
-      <c r="E16" s="117"/>
+      <c r="E16" s="116"/>
     </row>
     <row r="17" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A17" s="114">
+      <c r="A17" s="113">
         <v>615</v>
       </c>
-      <c r="B17" s="118" t="s">
+      <c r="B17" s="117" t="s">
         <v>85</v>
       </c>
       <c r="C17" s="105" t="s">
@@ -7730,13 +7883,13 @@
       <c r="D17" s="105" t="s">
         <v>86</v>
       </c>
-      <c r="E17" s="117"/>
+      <c r="E17" s="116"/>
     </row>
     <row r="18" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A18" s="114">
+      <c r="A18" s="113">
         <v>616</v>
       </c>
-      <c r="B18" s="118" t="s">
+      <c r="B18" s="117" t="s">
         <v>87</v>
       </c>
       <c r="C18" s="105" t="s">
@@ -7745,13 +7898,13 @@
       <c r="D18" s="105" t="s">
         <v>88</v>
       </c>
-      <c r="E18" s="117"/>
+      <c r="E18" s="116"/>
     </row>
     <row r="19" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A19" s="114">
+      <c r="A19" s="113">
         <v>617</v>
       </c>
-      <c r="B19" s="118" t="s">
+      <c r="B19" s="117" t="s">
         <v>89</v>
       </c>
       <c r="C19" s="105" t="s">
@@ -7760,13 +7913,13 @@
       <c r="D19" s="105" t="s">
         <v>90</v>
       </c>
-      <c r="E19" s="117"/>
+      <c r="E19" s="116"/>
     </row>
     <row r="20" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A20" s="114">
+      <c r="A20" s="113">
         <v>618</v>
       </c>
-      <c r="B20" s="118" t="s">
+      <c r="B20" s="117" t="s">
         <v>91</v>
       </c>
       <c r="C20" s="105" t="s">
@@ -7775,13 +7928,13 @@
       <c r="D20" s="105" t="s">
         <v>92</v>
       </c>
-      <c r="E20" s="117"/>
+      <c r="E20" s="116"/>
     </row>
     <row r="21" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A21" s="114">
+      <c r="A21" s="113">
         <v>619</v>
       </c>
-      <c r="B21" s="118" t="s">
+      <c r="B21" s="117" t="s">
         <v>93</v>
       </c>
       <c r="C21" s="105" t="s">
@@ -7790,13 +7943,13 @@
       <c r="D21" s="105" t="s">
         <v>94</v>
       </c>
-      <c r="E21" s="117"/>
+      <c r="E21" s="116"/>
     </row>
     <row r="22" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A22" s="114">
+      <c r="A22" s="113">
         <v>620</v>
       </c>
-      <c r="B22" s="118" t="s">
+      <c r="B22" s="117" t="s">
         <v>95</v>
       </c>
       <c r="C22" s="105" t="s">
@@ -7805,13 +7958,13 @@
       <c r="D22" s="105" t="s">
         <v>96</v>
       </c>
-      <c r="E22" s="117"/>
+      <c r="E22" s="116"/>
     </row>
     <row r="23" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A23" s="114">
+      <c r="A23" s="113">
         <v>621</v>
       </c>
-      <c r="B23" s="118" t="s">
+      <c r="B23" s="117" t="s">
         <v>70</v>
       </c>
       <c r="C23" s="105" t="s">
@@ -7820,13 +7973,13 @@
       <c r="D23" s="105" t="s">
         <v>72</v>
       </c>
-      <c r="E23" s="117"/>
+      <c r="E23" s="116"/>
     </row>
     <row r="24" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A24" s="119">
+      <c r="A24" s="118">
         <v>622</v>
       </c>
-      <c r="B24" s="118" t="s">
+      <c r="B24" s="117" t="s">
         <v>185</v>
       </c>
       <c r="C24" s="105" t="s">
@@ -7835,13 +7988,13 @@
       <c r="D24" s="105" t="s">
         <v>186</v>
       </c>
-      <c r="E24" s="117"/>
+      <c r="E24" s="116"/>
     </row>
     <row r="25" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A25" s="119">
+      <c r="A25" s="118">
         <v>623</v>
       </c>
-      <c r="B25" s="118" t="s">
+      <c r="B25" s="117" t="s">
         <v>187</v>
       </c>
       <c r="C25" s="105" t="s">
@@ -7850,13 +8003,13 @@
       <c r="D25" s="105" t="s">
         <v>188</v>
       </c>
-      <c r="E25" s="117"/>
+      <c r="E25" s="116"/>
     </row>
     <row r="26" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A26" s="119">
+      <c r="A26" s="118">
         <v>624</v>
       </c>
-      <c r="B26" s="118" t="s">
+      <c r="B26" s="117" t="s">
         <v>189</v>
       </c>
       <c r="C26" s="105" t="s">
@@ -7865,13 +8018,13 @@
       <c r="D26" s="105" t="s">
         <v>175</v>
       </c>
-      <c r="E26" s="117"/>
+      <c r="E26" s="116"/>
     </row>
     <row r="27" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A27" s="119">
+      <c r="A27" s="118">
         <v>625</v>
       </c>
-      <c r="B27" s="118" t="s">
+      <c r="B27" s="117" t="s">
         <v>190</v>
       </c>
       <c r="C27" s="105" t="s">
@@ -7880,19 +8033,19 @@
       <c r="D27" s="105" t="s">
         <v>191</v>
       </c>
-      <c r="E27" s="117"/>
+      <c r="E27" s="116"/>
     </row>
     <row r="28" s="107" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A28" s="110" t="s">
+      <c r="A28" s="109" t="s">
         <v>97</v>
       </c>
-      <c r="B28" s="111"/>
-      <c r="C28" s="112"/>
-      <c r="D28" s="112"/>
-      <c r="E28" s="113"/>
+      <c r="B28" s="110"/>
+      <c r="C28" s="111"/>
+      <c r="D28" s="111"/>
+      <c r="E28" s="112"/>
     </row>
     <row r="29" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A29" s="114">
+      <c r="A29" s="113">
         <v>601</v>
       </c>
       <c r="B29" s="105" t="s">
@@ -7907,7 +8060,7 @@
       <c r="E29" s="106"/>
     </row>
     <row r="30" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A30" s="114">
+      <c r="A30" s="113">
         <v>602</v>
       </c>
       <c r="B30" s="105" t="s">
@@ -7922,7 +8075,7 @@
       <c r="E30" s="106"/>
     </row>
     <row r="31" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A31" s="114">
+      <c r="A31" s="113">
         <v>603</v>
       </c>
       <c r="B31" s="105" t="s">
@@ -7937,7 +8090,7 @@
       <c r="E31" s="106"/>
     </row>
     <row r="32" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A32" s="114">
+      <c r="A32" s="113">
         <v>604</v>
       </c>
       <c r="B32" s="105" t="s">
@@ -7952,13 +8105,13 @@
       <c r="E32" s="106"/>
     </row>
     <row r="33" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A33" s="114">
+      <c r="A33" s="113">
         <v>605</v>
       </c>
       <c r="B33" s="105" t="s">
         <v>180</v>
       </c>
-      <c r="C33" s="116" t="s">
+      <c r="C33" s="115" t="s">
         <v>181</v>
       </c>
       <c r="D33" s="105" t="s">
@@ -7967,13 +8120,13 @@
       <c r="E33" s="106"/>
     </row>
     <row r="34" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A34" s="114">
+      <c r="A34" s="113">
         <v>606</v>
       </c>
       <c r="B34" s="105" t="s">
         <v>183</v>
       </c>
-      <c r="C34" s="116" t="s">
+      <c r="C34" s="115" t="s">
         <v>181</v>
       </c>
       <c r="D34" s="105" t="s">
@@ -7982,25 +8135,25 @@
       <c r="E34" s="106"/>
     </row>
     <row r="35" ht="18.75" spans="1:5">
-      <c r="A35" s="114">
+      <c r="A35" s="113">
         <v>607</v>
       </c>
       <c r="B35" s="105" t="s">
         <v>65</v>
       </c>
-      <c r="C35" s="116" t="s">
+      <c r="C35" s="115" t="s">
         <v>66</v>
       </c>
       <c r="D35" s="105" t="s">
         <v>67</v>
       </c>
-      <c r="E35" s="117"/>
+      <c r="E35" s="116"/>
     </row>
     <row r="36" ht="18.75" spans="1:5">
-      <c r="A36" s="114">
+      <c r="A36" s="113">
         <v>608</v>
       </c>
-      <c r="B36" s="118" t="s">
+      <c r="B36" s="117" t="s">
         <v>98</v>
       </c>
       <c r="C36" s="105" t="s">
@@ -8009,10 +8162,10 @@
       <c r="D36" s="105" t="s">
         <v>99</v>
       </c>
-      <c r="E36" s="117"/>
+      <c r="E36" s="116"/>
     </row>
     <row r="37" ht="18.75" spans="1:5">
-      <c r="A37" s="114">
+      <c r="A37" s="113">
         <v>609</v>
       </c>
       <c r="B37" s="105" t="s">
@@ -8024,25 +8177,25 @@
       <c r="D37" s="105" t="s">
         <v>69</v>
       </c>
-      <c r="E37" s="117"/>
+      <c r="E37" s="116"/>
     </row>
     <row r="38" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A38" s="114">
+      <c r="A38" s="113">
         <v>610</v>
       </c>
       <c r="B38" s="105" t="s">
         <v>192</v>
       </c>
-      <c r="C38" s="116" t="s">
+      <c r="C38" s="115" t="s">
         <v>66</v>
       </c>
       <c r="D38" s="105" t="s">
         <v>193</v>
       </c>
-      <c r="E38" s="117"/>
+      <c r="E38" s="116"/>
     </row>
     <row r="39" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A39" s="114">
+      <c r="A39" s="113">
         <v>611</v>
       </c>
       <c r="B39" s="105" t="s">
@@ -8054,13 +8207,13 @@
       <c r="D39" s="105" t="s">
         <v>195</v>
       </c>
-      <c r="E39" s="117"/>
+      <c r="E39" s="116"/>
     </row>
     <row r="40" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A40" s="114">
+      <c r="A40" s="113">
         <v>612</v>
       </c>
-      <c r="B40" s="118" t="s">
+      <c r="B40" s="117" t="s">
         <v>185</v>
       </c>
       <c r="C40" s="105" t="s">
@@ -8069,13 +8222,13 @@
       <c r="D40" s="105" t="s">
         <v>186</v>
       </c>
-      <c r="E40" s="117"/>
+      <c r="E40" s="116"/>
     </row>
     <row r="41" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A41" s="114">
+      <c r="A41" s="113">
         <v>613</v>
       </c>
-      <c r="B41" s="118" t="s">
+      <c r="B41" s="117" t="s">
         <v>189</v>
       </c>
       <c r="C41" s="105" t="s">
@@ -8084,13 +8237,13 @@
       <c r="D41" s="105" t="s">
         <v>175</v>
       </c>
-      <c r="E41" s="117"/>
+      <c r="E41" s="116"/>
     </row>
     <row r="42" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A42" s="114">
+      <c r="A42" s="113">
         <v>614</v>
       </c>
-      <c r="B42" s="118" t="s">
+      <c r="B42" s="117" t="s">
         <v>190</v>
       </c>
       <c r="C42" s="105" t="s">
@@ -8099,13 +8252,13 @@
       <c r="D42" s="105" t="s">
         <v>191</v>
       </c>
-      <c r="E42" s="117"/>
+      <c r="E42" s="116"/>
     </row>
     <row r="43" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A43" s="114">
+      <c r="A43" s="113">
         <v>615</v>
       </c>
-      <c r="B43" s="118" t="s">
+      <c r="B43" s="117" t="s">
         <v>187</v>
       </c>
       <c r="C43" s="105" t="s">
@@ -8114,19 +8267,19 @@
       <c r="D43" s="105" t="s">
         <v>188</v>
       </c>
-      <c r="E43" s="117"/>
+      <c r="E43" s="116"/>
     </row>
     <row r="44" s="107" customFormat="1" ht="18.75" spans="1:5">
-      <c r="A44" s="110" t="s">
+      <c r="A44" s="109" t="s">
         <v>100</v>
       </c>
-      <c r="B44" s="111"/>
-      <c r="C44" s="112"/>
-      <c r="D44" s="112"/>
-      <c r="E44" s="113"/>
+      <c r="B44" s="110"/>
+      <c r="C44" s="111"/>
+      <c r="D44" s="111"/>
+      <c r="E44" s="112"/>
     </row>
     <row r="45" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A45" s="114">
+      <c r="A45" s="113">
         <v>601</v>
       </c>
       <c r="B45" s="105" t="s">
@@ -8141,7 +8294,7 @@
       <c r="E45" s="106"/>
     </row>
     <row r="46" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A46" s="114">
+      <c r="A46" s="113">
         <v>602</v>
       </c>
       <c r="B46" s="105" t="s">
@@ -8156,7 +8309,7 @@
       <c r="E46" s="106"/>
     </row>
     <row r="47" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A47" s="114">
+      <c r="A47" s="113">
         <v>603</v>
       </c>
       <c r="B47" s="105" t="s">
@@ -8171,7 +8324,7 @@
       <c r="E47" s="106"/>
     </row>
     <row r="48" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A48" s="114">
+      <c r="A48" s="113">
         <v>604</v>
       </c>
       <c r="B48" s="105" t="s">
@@ -8186,7 +8339,7 @@
       <c r="E48" s="106"/>
     </row>
     <row r="49" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A49" s="114">
+      <c r="A49" s="113">
         <v>605</v>
       </c>
       <c r="B49" s="105" t="s">
@@ -8201,7 +8354,7 @@
       <c r="E49" s="106"/>
     </row>
     <row r="50" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A50" s="114">
+      <c r="A50" s="113">
         <v>606</v>
       </c>
       <c r="B50" s="105" t="s">
@@ -8216,7 +8369,7 @@
       <c r="E50" s="106"/>
     </row>
     <row r="51" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A51" s="114">
+      <c r="A51" s="113">
         <v>607</v>
       </c>
       <c r="B51" s="105" t="s">
@@ -8231,7 +8384,7 @@
       <c r="E51" s="106"/>
     </row>
     <row r="52" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A52" s="114">
+      <c r="A52" s="113">
         <v>608</v>
       </c>
       <c r="B52" s="105" t="s">
@@ -8246,13 +8399,13 @@
       <c r="E52" s="106"/>
     </row>
     <row r="53" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A53" s="114">
+      <c r="A53" s="113">
         <v>609</v>
       </c>
       <c r="B53" s="105" t="s">
         <v>204</v>
       </c>
-      <c r="C53" s="116" t="s">
+      <c r="C53" s="115" t="s">
         <v>181</v>
       </c>
       <c r="D53" s="105" t="s">
@@ -8261,13 +8414,13 @@
       <c r="E53" s="106"/>
     </row>
     <row r="54" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A54" s="114">
+      <c r="A54" s="113">
         <v>610</v>
       </c>
       <c r="B54" s="105" t="s">
         <v>206</v>
       </c>
-      <c r="C54" s="116" t="s">
+      <c r="C54" s="115" t="s">
         <v>181</v>
       </c>
       <c r="D54" s="105" t="s">
@@ -8276,13 +8429,13 @@
       <c r="E54" s="106"/>
     </row>
     <row r="55" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A55" s="114">
+      <c r="A55" s="113">
         <v>611</v>
       </c>
       <c r="B55" s="105" t="s">
         <v>208</v>
       </c>
-      <c r="C55" s="116" t="s">
+      <c r="C55" s="115" t="s">
         <v>181</v>
       </c>
       <c r="D55" s="105" t="s">
@@ -8291,13 +8444,13 @@
       <c r="E55" s="106"/>
     </row>
     <row r="56" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A56" s="114">
+      <c r="A56" s="113">
         <v>612</v>
       </c>
       <c r="B56" s="105" t="s">
         <v>210</v>
       </c>
-      <c r="C56" s="116" t="s">
+      <c r="C56" s="115" t="s">
         <v>181</v>
       </c>
       <c r="D56" s="105" t="s">
@@ -8306,13 +8459,13 @@
       <c r="E56" s="106"/>
     </row>
     <row r="57" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A57" s="114">
+      <c r="A57" s="113">
         <v>613</v>
       </c>
       <c r="B57" s="105" t="s">
         <v>212</v>
       </c>
-      <c r="C57" s="116" t="s">
+      <c r="C57" s="115" t="s">
         <v>66</v>
       </c>
       <c r="D57" s="105" t="s">
@@ -8321,13 +8474,13 @@
       <c r="E57" s="106"/>
     </row>
     <row r="58" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A58" s="114">
+      <c r="A58" s="113">
         <v>614</v>
       </c>
       <c r="B58" s="105" t="s">
         <v>214</v>
       </c>
-      <c r="C58" s="116" t="s">
+      <c r="C58" s="115" t="s">
         <v>66</v>
       </c>
       <c r="D58" s="105" t="s">
@@ -8336,13 +8489,13 @@
       <c r="E58" s="106"/>
     </row>
     <row r="59" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A59" s="114">
+      <c r="A59" s="113">
         <v>615</v>
       </c>
       <c r="B59" s="105" t="s">
         <v>216</v>
       </c>
-      <c r="C59" s="116" t="s">
+      <c r="C59" s="115" t="s">
         <v>66</v>
       </c>
       <c r="D59" s="105" t="s">
@@ -8351,13 +8504,13 @@
       <c r="E59" s="106"/>
     </row>
     <row r="60" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A60" s="114">
+      <c r="A60" s="113">
         <v>616</v>
       </c>
       <c r="B60" s="105" t="s">
         <v>218</v>
       </c>
-      <c r="C60" s="116" t="s">
+      <c r="C60" s="115" t="s">
         <v>66</v>
       </c>
       <c r="D60" s="105" t="s">
@@ -8366,13 +8519,13 @@
       <c r="E60" s="106"/>
     </row>
     <row r="61" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A61" s="114">
+      <c r="A61" s="113">
         <v>617</v>
       </c>
       <c r="B61" s="105" t="s">
         <v>220</v>
       </c>
-      <c r="C61" s="116" t="s">
+      <c r="C61" s="115" t="s">
         <v>66</v>
       </c>
       <c r="D61" s="105" t="s">
@@ -8381,13 +8534,13 @@
       <c r="E61" s="106"/>
     </row>
     <row r="62" ht="18.9" customHeight="1" spans="1:5">
-      <c r="A62" s="114">
+      <c r="A62" s="113">
         <v>618</v>
       </c>
       <c r="B62" s="105" t="s">
         <v>222</v>
       </c>
-      <c r="C62" s="116" t="s">
+      <c r="C62" s="115" t="s">
         <v>66</v>
       </c>
       <c r="D62" s="105" t="s">
@@ -8396,232 +8549,232 @@
       <c r="E62" s="106"/>
     </row>
     <row r="63" ht="18.75" spans="1:5">
-      <c r="A63" s="114">
+      <c r="A63" s="113">
         <v>619</v>
       </c>
       <c r="B63" s="105" t="s">
         <v>109</v>
       </c>
-      <c r="C63" s="116" t="s">
+      <c r="C63" s="115" t="s">
         <v>66</v>
       </c>
       <c r="D63" s="105" t="s">
         <v>110</v>
       </c>
-      <c r="E63" s="117"/>
+      <c r="E63" s="116"/>
     </row>
     <row r="64" ht="18.75" spans="1:5">
-      <c r="A64" s="114">
+      <c r="A64" s="113">
         <v>620</v>
       </c>
       <c r="B64" s="105" t="s">
         <v>131</v>
       </c>
-      <c r="C64" s="116" t="s">
+      <c r="C64" s="115" t="s">
         <v>66</v>
       </c>
       <c r="D64" s="105" t="s">
         <v>132</v>
       </c>
-      <c r="E64" s="117"/>
+      <c r="E64" s="116"/>
     </row>
     <row r="65" ht="18.75" spans="1:5">
-      <c r="A65" s="114">
+      <c r="A65" s="113">
         <v>621</v>
       </c>
       <c r="B65" s="105" t="s">
         <v>111</v>
       </c>
-      <c r="C65" s="116" t="s">
+      <c r="C65" s="115" t="s">
         <v>66</v>
       </c>
       <c r="D65" s="105" t="s">
         <v>112</v>
       </c>
-      <c r="E65" s="117"/>
+      <c r="E65" s="116"/>
     </row>
     <row r="66" ht="18.75" spans="1:5">
-      <c r="A66" s="114">
+      <c r="A66" s="113">
         <v>622</v>
       </c>
       <c r="B66" s="105" t="s">
         <v>133</v>
       </c>
-      <c r="C66" s="116" t="s">
+      <c r="C66" s="115" t="s">
         <v>66</v>
       </c>
       <c r="D66" s="105" t="s">
         <v>134</v>
       </c>
-      <c r="E66" s="117"/>
+      <c r="E66" s="116"/>
     </row>
     <row r="67" ht="18.75" spans="1:5">
-      <c r="A67" s="114">
+      <c r="A67" s="113">
         <v>623</v>
       </c>
       <c r="B67" s="105" t="s">
         <v>113</v>
       </c>
-      <c r="C67" s="116" t="s">
+      <c r="C67" s="115" t="s">
         <v>66</v>
       </c>
       <c r="D67" s="105" t="s">
         <v>114</v>
       </c>
-      <c r="E67" s="117"/>
+      <c r="E67" s="116"/>
     </row>
     <row r="68" ht="18.75" spans="1:5">
-      <c r="A68" s="114">
+      <c r="A68" s="113">
         <v>624</v>
       </c>
       <c r="B68" s="105" t="s">
         <v>135</v>
       </c>
-      <c r="C68" s="116" t="s">
+      <c r="C68" s="115" t="s">
         <v>66</v>
       </c>
       <c r="D68" s="105" t="s">
         <v>136</v>
       </c>
-      <c r="E68" s="117"/>
+      <c r="E68" s="116"/>
     </row>
     <row r="69" ht="18.75" spans="1:5">
-      <c r="A69" s="114">
+      <c r="A69" s="113">
         <v>625</v>
       </c>
       <c r="B69" s="105" t="s">
         <v>115</v>
       </c>
-      <c r="C69" s="116" t="s">
+      <c r="C69" s="115" t="s">
         <v>66</v>
       </c>
       <c r="D69" s="105" t="s">
         <v>116</v>
       </c>
-      <c r="E69" s="117"/>
+      <c r="E69" s="116"/>
     </row>
     <row r="70" ht="18.75" spans="1:5">
-      <c r="A70" s="114">
+      <c r="A70" s="113">
         <v>626</v>
       </c>
       <c r="B70" s="105" t="s">
         <v>137</v>
       </c>
-      <c r="C70" s="116" t="s">
+      <c r="C70" s="115" t="s">
         <v>66</v>
       </c>
       <c r="D70" s="105" t="s">
         <v>138</v>
       </c>
-      <c r="E70" s="117"/>
+      <c r="E70" s="116"/>
     </row>
     <row r="71" ht="18.75" spans="1:5">
-      <c r="A71" s="114">
+      <c r="A71" s="113">
         <v>627</v>
       </c>
       <c r="B71" s="105" t="s">
         <v>117</v>
       </c>
-      <c r="C71" s="116" t="s">
+      <c r="C71" s="115" t="s">
         <v>66</v>
       </c>
       <c r="D71" s="105" t="s">
         <v>118</v>
       </c>
-      <c r="E71" s="117"/>
+      <c r="E71" s="116"/>
     </row>
     <row r="72" ht="18.75" spans="1:5">
-      <c r="A72" s="114">
+      <c r="A72" s="113">
         <v>628</v>
       </c>
       <c r="B72" s="105" t="s">
         <v>139</v>
       </c>
-      <c r="C72" s="116" t="s">
+      <c r="C72" s="115" t="s">
         <v>66</v>
       </c>
       <c r="D72" s="105" t="s">
         <v>140</v>
       </c>
-      <c r="E72" s="117"/>
+      <c r="E72" s="116"/>
     </row>
     <row r="73" ht="18.75" spans="1:5">
-      <c r="A73" s="114">
+      <c r="A73" s="113">
         <v>629</v>
       </c>
       <c r="B73" s="105" t="s">
         <v>119</v>
       </c>
-      <c r="C73" s="116" t="s">
+      <c r="C73" s="115" t="s">
         <v>66</v>
       </c>
       <c r="D73" s="105" t="s">
         <v>120</v>
       </c>
-      <c r="E73" s="117"/>
+      <c r="E73" s="116"/>
     </row>
     <row r="74" ht="18.75" spans="1:5">
-      <c r="A74" s="114">
+      <c r="A74" s="113">
         <v>630</v>
       </c>
       <c r="B74" s="105" t="s">
         <v>141</v>
       </c>
-      <c r="C74" s="116" t="s">
+      <c r="C74" s="115" t="s">
         <v>66</v>
       </c>
       <c r="D74" s="105" t="s">
         <v>142</v>
       </c>
-      <c r="E74" s="117"/>
+      <c r="E74" s="116"/>
     </row>
     <row r="75" ht="18.75" spans="1:5">
-      <c r="A75" s="114">
+      <c r="A75" s="113">
         <v>631</v>
       </c>
       <c r="B75" s="105" t="s">
         <v>121</v>
       </c>
-      <c r="C75" s="116" t="s">
+      <c r="C75" s="115" t="s">
         <v>66</v>
       </c>
       <c r="D75" s="105" t="s">
         <v>122</v>
       </c>
-      <c r="E75" s="117"/>
+      <c r="E75" s="116"/>
     </row>
     <row r="76" ht="18.75" spans="1:5">
-      <c r="A76" s="114">
+      <c r="A76" s="113">
         <v>632</v>
       </c>
       <c r="B76" s="105" t="s">
         <v>143</v>
       </c>
-      <c r="C76" s="116" t="s">
+      <c r="C76" s="115" t="s">
         <v>66</v>
       </c>
       <c r="D76" s="105" t="s">
         <v>144</v>
       </c>
-      <c r="E76" s="117"/>
+      <c r="E76" s="116"/>
     </row>
     <row r="77" ht="18.75" spans="1:5">
-      <c r="A77" s="114">
+      <c r="A77" s="113">
         <v>633</v>
       </c>
       <c r="B77" s="105" t="s">
         <v>145</v>
       </c>
-      <c r="C77" s="116" t="s">
+      <c r="C77" s="115" t="s">
         <v>66</v>
       </c>
       <c r="D77" s="105" t="s">
         <v>146</v>
       </c>
-      <c r="E77" s="117"/>
+      <c r="E77" s="116"/>
     </row>
     <row r="78" ht="18.75" spans="1:5">
-      <c r="A78" s="114">
+      <c r="A78" s="113">
         <v>634</v>
       </c>
       <c r="B78" s="105" t="s">
@@ -8633,10 +8786,10 @@
       <c r="D78" s="105" t="s">
         <v>148</v>
       </c>
-      <c r="E78" s="117"/>
+      <c r="E78" s="116"/>
     </row>
     <row r="79" ht="18.75" spans="1:5">
-      <c r="A79" s="114">
+      <c r="A79" s="113">
         <v>635</v>
       </c>
       <c r="B79" s="105" t="s">
@@ -8648,7 +8801,7 @@
       <c r="D79" s="105" t="s">
         <v>224</v>
       </c>
-      <c r="E79" s="117"/>
+      <c r="E79" s="116"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>